<commit_message>
updating assertions for webflux-demo
</commit_message>
<xml_diff>
--- a/src/test/resources/auto-test-resources/webflux-demo-unit-resources.xlsx
+++ b/src/test/resources/auto-test-resources/webflux-demo-unit-resources.xlsx
@@ -3769,7 +3769,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3785,6 +3785,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -20057,8 +20060,8 @@
       <c r="E457" s="4" t="s">
         <v>1023</v>
       </c>
-      <c r="F457" s="2" t="s">
-        <v>15</v>
+      <c r="F457" s="6" t="s">
+        <v>184</v>
       </c>
       <c r="G457" s="5" t="s">
         <v>1042</v>
@@ -20365,8 +20368,8 @@
       <c r="E464" s="4" t="s">
         <v>1023</v>
       </c>
-      <c r="F464" s="2" t="s">
-        <v>15</v>
+      <c r="F464" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="G464" s="5" t="s">
         <v>28</v>
@@ -20629,8 +20632,8 @@
       <c r="E470" s="4" t="s">
         <v>1079</v>
       </c>
-      <c r="F470" s="2" t="s">
-        <v>15</v>
+      <c r="F470" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="G470" s="5" t="s">
         <v>28</v>
@@ -20805,8 +20808,8 @@
       <c r="E474" s="4" t="s">
         <v>1063</v>
       </c>
-      <c r="F474" s="2" t="s">
-        <v>15</v>
+      <c r="F474" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="G474" s="5" t="s">
         <v>28</v>
@@ -20849,8 +20852,8 @@
       <c r="E475" s="4" t="s">
         <v>1023</v>
       </c>
-      <c r="F475" s="2" t="s">
-        <v>15</v>
+      <c r="F475" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="G475" s="5" t="s">
         <v>28</v>

</xml_diff>